<commit_message>
Day 3 sprint backlog
Tasks removed due to merge tasks taking longer to complete than expected
</commit_message>
<xml_diff>
--- a/Sprint 2/Sprint Backlog/Sprint 2 backlog.xlsx
+++ b/Sprint 2/Sprint Backlog/Sprint 2 backlog.xlsx
@@ -7,16 +7,16 @@
     <sheet state="visible" name="-Disclaimer-" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="YesNo">'Agile Product Backlog'!$O$5:$O$14</definedName>
-    <definedName name="Priority">'Agile Product Backlog'!$P$5:$P$20</definedName>
-    <definedName name="Status">'Agile Product Backlog'!$Q$5:$Q$20</definedName>
+    <definedName name="YesNo">'Agile Product Backlog'!$O$5:$O$13</definedName>
+    <definedName name="Priority">'Agile Product Backlog'!$P$5:$P$14</definedName>
+    <definedName name="Status">'Agile Product Backlog'!$Q$5:$Q$14</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
   <si>
     <t>SPRINT BACKLOG</t>
   </si>
@@ -122,7 +122,13 @@
     <t>Merge HTML front end with back end search function: search by code, distance, procedure</t>
   </si>
   <si>
+    <t>Ben, Joel</t>
+  </si>
+  <si>
     <t>Merge HTML front end with back end search function: restrict search by distance, price</t>
+  </si>
+  <si>
+    <t>Jodie, Tony, Dimitar</t>
   </si>
   <si>
     <t>Merge HTML front end with back end search function: order by price, distance</t>
@@ -150,51 +156,6 @@
   </si>
   <si>
     <t>As a user, I can use my device's location as an input for the search, so that I can save time and don't need to know the address, state or zip code location I am currently at</t>
-  </si>
-  <si>
-    <t>Dimitar</t>
-  </si>
-  <si>
-    <t>Add screen reader functionality</t>
-  </si>
-  <si>
-    <t>As a user, I can use a screen reader to read the page, so that I can still use the website if I have a visual imparement</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Medium</t>
-  </si>
-  <si>
-    <t>Add text resize options</t>
-  </si>
-  <si>
-    <t>As a user, I can resize the text, so that I can make it bigger/smaller to suit my needs</t>
-  </si>
-  <si>
-    <t>Add text/image colour options</t>
-  </si>
-  <si>
-    <t>As a user, I can change the colours used on the web page, so that can still use the website if I have a visual imparement</t>
-  </si>
-  <si>
-    <t>Create a function to add data to the existing data set</t>
-  </si>
-  <si>
-    <t>As a Centers for Medicare &amp; Medicaid manager, I can load new data to the existing dataset through the website, so that; when the dataset is updated, I can easily update the databse</t>
-  </si>
-  <si>
-    <t>Ben</t>
-  </si>
-  <si>
-    <t>Create a function to delete the existing data set</t>
-  </si>
-  <si>
-    <t>As a Centers for Medicare &amp; Medicaid manager, I can delete data from the existing dataset through the website, so that; when the dataset is updated, I can easily update the databse</t>
-  </si>
-  <si>
-    <t>Create a function to edit the existing data set</t>
   </si>
   <si>
     <t>Merge all tasks together</t>
@@ -287,7 +248,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="7">
     <border/>
     <border>
       <left/>
@@ -348,41 +309,11 @@
         <color rgb="FFBFBFBF"/>
       </bottom>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFBFBFBF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFBFBFBF"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFBFBFBF"/>
-      </top>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFBFBFBF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFBFBFBF"/>
-      </right>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFBFBFBF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFBFBFBF"/>
-      </right>
-      <bottom style="thin">
-        <color rgb="FFBFBFBF"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="24">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -445,15 +376,6 @@
     <xf borderId="6" fillId="3" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="3" fillId="4" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -864,7 +786,7 @@
         <v>20</v>
       </c>
       <c r="I4" s="16">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="J4" s="17">
         <v>43923.0</v>
@@ -1093,7 +1015,7 @@
         <v>3</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="I8" s="16">
         <v>5.0</v>
@@ -1135,7 +1057,7 @@
       <c r="A9" s="1"/>
       <c r="B9" s="15"/>
       <c r="C9" s="16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D9" s="16"/>
       <c r="E9" s="16">
@@ -1149,7 +1071,7 @@
         <v>2.25</v>
       </c>
       <c r="H9" s="16" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="I9" s="16">
         <v>5.0</v>
@@ -1191,7 +1113,7 @@
       <c r="A10" s="1"/>
       <c r="B10" s="15"/>
       <c r="C10" s="16" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D10" s="16"/>
       <c r="E10" s="16">
@@ -1205,7 +1127,7 @@
         <v>2.25</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="I10" s="16">
         <v>5.0</v>
@@ -1247,7 +1169,7 @@
       <c r="A11" s="1"/>
       <c r="B11" s="15"/>
       <c r="C11" s="16" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D11" s="16"/>
       <c r="E11" s="16">
@@ -1258,7 +1180,7 @@
       </c>
       <c r="G11" s="16"/>
       <c r="H11" s="16" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I11" s="16">
         <v>3.0</v>
@@ -1300,10 +1222,10 @@
       <c r="A12" s="1"/>
       <c r="B12" s="16"/>
       <c r="C12" s="16" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E12" s="16">
         <v>3.0</v>
@@ -1312,11 +1234,11 @@
         <v>7.0</v>
       </c>
       <c r="G12" s="16">
-        <f t="shared" ref="G12:G20" si="2">F12/E12</f>
+        <f t="shared" ref="G12:G14" si="2">F12/E12</f>
         <v>2.333333333</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I12" s="16">
         <v>2.0</v>
@@ -1328,7 +1250,7 @@
         <v>43923.0</v>
       </c>
       <c r="L12" s="16" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="M12" s="18"/>
       <c r="N12" s="7"/>
@@ -1358,10 +1280,10 @@
       <c r="A13" s="1"/>
       <c r="B13" s="15"/>
       <c r="C13" s="16" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E13" s="16">
         <v>3.0</v>
@@ -1374,7 +1296,7 @@
         <v>1.666666667</v>
       </c>
       <c r="H13" s="16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I13" s="16">
         <v>1.0</v>
@@ -1386,7 +1308,7 @@
         <v>43984.0</v>
       </c>
       <c r="L13" s="16" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="M13" s="18"/>
       <c r="N13" s="7"/>
@@ -1412,51 +1334,43 @@
       <c r="AH13" s="7"/>
       <c r="AI13" s="7"/>
     </row>
-    <row r="14" ht="54.0" customHeight="1">
+    <row r="14" ht="46.5" customHeight="1">
       <c r="A14" s="1"/>
       <c r="B14" s="15"/>
       <c r="C14" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="23" t="s">
         <v>46</v>
       </c>
+      <c r="D14" s="16"/>
       <c r="E14" s="16">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="F14" s="16">
-        <v>4.0</v>
+        <v>10.0</v>
       </c>
       <c r="G14" s="16">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H14" s="16" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="I14" s="16">
-        <v>1.0</v>
+        <v>8.0</v>
       </c>
-      <c r="J14" s="17">
-        <v>43923.0</v>
+      <c r="J14" s="23">
+        <v>43984.0</v>
       </c>
-      <c r="K14" s="17">
-        <v>43953.0</v>
+      <c r="K14" s="23">
+        <v>44014.0</v>
       </c>
       <c r="L14" s="16" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="M14" s="18"/>
       <c r="N14" s="7"/>
-      <c r="O14" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="P14" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q14" s="22" t="s">
-        <v>21</v>
-      </c>
+      <c r="O14" s="22"/>
+      <c r="P14" s="22"/>
+      <c r="Q14" s="22"/>
       <c r="R14" s="7"/>
       <c r="S14" s="7"/>
       <c r="T14" s="7"/>
@@ -1476,45 +1390,12 @@
       <c r="AH14" s="7"/>
       <c r="AI14" s="7"/>
     </row>
-    <row r="15" ht="59.25" customHeight="1">
+    <row r="15" ht="9.75" customHeight="1">
       <c r="A15" s="1"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="E15" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="F15" s="16">
-        <v>4.0</v>
-      </c>
-      <c r="G15" s="16">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="H15" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="I15" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="J15" s="17">
-        <v>43923.0</v>
-      </c>
-      <c r="K15" s="17">
-        <v>43953.0</v>
-      </c>
-      <c r="L15" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="M15" s="18"/>
       <c r="N15" s="7"/>
-      <c r="O15" s="22"/>
-      <c r="P15" s="22"/>
-      <c r="Q15" s="22"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
       <c r="R15" s="7"/>
       <c r="S15" s="7"/>
       <c r="T15" s="7"/>
@@ -1534,45 +1415,12 @@
       <c r="AH15" s="7"/>
       <c r="AI15" s="7"/>
     </row>
-    <row r="16" ht="45.75" customHeight="1">
+    <row r="16" ht="12.75" customHeight="1">
       <c r="A16" s="1"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="D16" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="E16" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="F16" s="16">
-        <v>4.0</v>
-      </c>
-      <c r="G16" s="16">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="H16" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="I16" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="J16" s="17">
-        <v>43923.0</v>
-      </c>
-      <c r="K16" s="17">
-        <v>43953.0</v>
-      </c>
-      <c r="L16" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="M16" s="18"/>
       <c r="N16" s="7"/>
-      <c r="O16" s="22"/>
-      <c r="P16" s="22"/>
-      <c r="Q16" s="22"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
       <c r="R16" s="7"/>
       <c r="S16" s="7"/>
       <c r="T16" s="7"/>
@@ -1592,45 +1440,12 @@
       <c r="AH16" s="7"/>
       <c r="AI16" s="7"/>
     </row>
-    <row r="17" ht="63.0" customHeight="1">
+    <row r="17" ht="12.75" customHeight="1">
       <c r="A17" s="1"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" s="16">
-        <v>2.0</v>
-      </c>
-      <c r="F17" s="16">
-        <v>3.0</v>
-      </c>
-      <c r="G17" s="16">
-        <f t="shared" si="2"/>
-        <v>1.5</v>
-      </c>
-      <c r="H17" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="I17" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="J17" s="17">
-        <v>43953.0</v>
-      </c>
-      <c r="K17" s="17">
-        <v>43984.0</v>
-      </c>
-      <c r="L17" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="M17" s="18"/>
       <c r="N17" s="7"/>
-      <c r="O17" s="22"/>
-      <c r="P17" s="22"/>
-      <c r="Q17" s="22"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
       <c r="R17" s="7"/>
       <c r="S17" s="7"/>
       <c r="T17" s="7"/>
@@ -1650,45 +1465,12 @@
       <c r="AH17" s="7"/>
       <c r="AI17" s="7"/>
     </row>
-    <row r="18" ht="60.75" customHeight="1">
+    <row r="18" ht="12.75" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="E18" s="16">
-        <v>2.0</v>
-      </c>
-      <c r="F18" s="16">
-        <v>3.0</v>
-      </c>
-      <c r="G18" s="16">
-        <f t="shared" si="2"/>
-        <v>1.5</v>
-      </c>
-      <c r="H18" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="I18" s="16">
-        <v>2.0</v>
-      </c>
-      <c r="J18" s="17">
-        <v>43953.0</v>
-      </c>
-      <c r="K18" s="17">
-        <v>43984.0</v>
-      </c>
-      <c r="L18" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="M18" s="18"/>
       <c r="N18" s="7"/>
-      <c r="O18" s="22"/>
-      <c r="P18" s="22"/>
-      <c r="Q18" s="22"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
       <c r="R18" s="7"/>
       <c r="S18" s="7"/>
       <c r="T18" s="7"/>
@@ -1708,45 +1490,12 @@
       <c r="AH18" s="7"/>
       <c r="AI18" s="7"/>
     </row>
-    <row r="19" ht="63.75" customHeight="1">
+    <row r="19" ht="12.75" customHeight="1">
       <c r="A19" s="1"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="E19" s="16">
-        <v>2.0</v>
-      </c>
-      <c r="F19" s="16">
-        <v>3.0</v>
-      </c>
-      <c r="G19" s="16">
-        <f t="shared" si="2"/>
-        <v>1.5</v>
-      </c>
-      <c r="H19" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="I19" s="16">
-        <v>2.0</v>
-      </c>
-      <c r="J19" s="17">
-        <v>43953.0</v>
-      </c>
-      <c r="K19" s="17">
-        <v>43984.0</v>
-      </c>
-      <c r="L19" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="M19" s="18"/>
       <c r="N19" s="7"/>
-      <c r="O19" s="22"/>
-      <c r="P19" s="22"/>
-      <c r="Q19" s="22"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
       <c r="R19" s="7"/>
       <c r="S19" s="7"/>
       <c r="T19" s="7"/>
@@ -1766,43 +1515,12 @@
       <c r="AH19" s="7"/>
       <c r="AI19" s="7"/>
     </row>
-    <row r="20" ht="46.5" customHeight="1">
+    <row r="20" ht="12.75" customHeight="1">
       <c r="A20" s="1"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16">
-        <v>2.0</v>
-      </c>
-      <c r="F20" s="16">
-        <v>10.0</v>
-      </c>
-      <c r="G20" s="16">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="H20" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="I20" s="16">
-        <v>8.0</v>
-      </c>
-      <c r="J20" s="26">
-        <v>43984.0</v>
-      </c>
-      <c r="K20" s="26">
-        <v>44014.0</v>
-      </c>
-      <c r="L20" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="M20" s="18"/>
       <c r="N20" s="7"/>
-      <c r="O20" s="22"/>
-      <c r="P20" s="22"/>
-      <c r="Q20" s="22"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
       <c r="R20" s="7"/>
       <c r="S20" s="7"/>
       <c r="T20" s="7"/>
@@ -1822,7 +1540,7 @@
       <c r="AH20" s="7"/>
       <c r="AI20" s="7"/>
     </row>
-    <row r="21" ht="9.75" customHeight="1">
+    <row r="21" ht="12.75" customHeight="1">
       <c r="A21" s="1"/>
       <c r="N21" s="7"/>
       <c r="O21" s="7"/>
@@ -1899,6 +1617,18 @@
     </row>
     <row r="24" ht="12.75" customHeight="1">
       <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
       <c r="N24" s="7"/>
       <c r="O24" s="7"/>
       <c r="P24" s="7"/>
@@ -1924,6 +1654,18 @@
     </row>
     <row r="25" ht="12.75" customHeight="1">
       <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
       <c r="N25" s="7"/>
       <c r="O25" s="7"/>
       <c r="P25" s="7"/>
@@ -1949,6 +1691,18 @@
     </row>
     <row r="26" ht="12.75" customHeight="1">
       <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
       <c r="N26" s="7"/>
       <c r="O26" s="7"/>
       <c r="P26" s="7"/>
@@ -1974,6 +1728,18 @@
     </row>
     <row r="27" ht="12.75" customHeight="1">
       <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
       <c r="N27" s="7"/>
       <c r="O27" s="7"/>
       <c r="P27" s="7"/>
@@ -1999,6 +1765,18 @@
     </row>
     <row r="28" ht="12.75" customHeight="1">
       <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
       <c r="N28" s="7"/>
       <c r="O28" s="7"/>
       <c r="P28" s="7"/>
@@ -2024,6 +1802,18 @@
     </row>
     <row r="29" ht="12.75" customHeight="1">
       <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
       <c r="N29" s="7"/>
       <c r="O29" s="7"/>
       <c r="P29" s="7"/>
@@ -2901,224 +2691,224 @@
     <row r="53" ht="12.75" customHeight="1">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
-      <c r="C53" s="7"/>
-      <c r="D53" s="7"/>
-      <c r="E53" s="7"/>
-      <c r="F53" s="7"/>
-      <c r="G53" s="7"/>
-      <c r="H53" s="7"/>
-      <c r="I53" s="7"/>
-      <c r="J53" s="7"/>
-      <c r="K53" s="7"/>
-      <c r="L53" s="7"/>
-      <c r="M53" s="7"/>
-      <c r="N53" s="7"/>
-      <c r="O53" s="7"/>
-      <c r="P53" s="7"/>
-      <c r="Q53" s="7"/>
-      <c r="R53" s="7"/>
-      <c r="S53" s="7"/>
-      <c r="T53" s="7"/>
-      <c r="U53" s="7"/>
-      <c r="V53" s="7"/>
-      <c r="W53" s="7"/>
-      <c r="X53" s="7"/>
-      <c r="Y53" s="7"/>
-      <c r="Z53" s="7"/>
-      <c r="AA53" s="7"/>
-      <c r="AB53" s="7"/>
-      <c r="AC53" s="7"/>
-      <c r="AD53" s="7"/>
-      <c r="AE53" s="7"/>
-      <c r="AF53" s="7"/>
-      <c r="AG53" s="7"/>
-      <c r="AH53" s="7"/>
-      <c r="AI53" s="7"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
+      <c r="L53" s="1"/>
+      <c r="M53" s="1"/>
+      <c r="N53" s="1"/>
+      <c r="O53" s="1"/>
+      <c r="P53" s="1"/>
+      <c r="Q53" s="1"/>
+      <c r="R53" s="1"/>
+      <c r="S53" s="1"/>
+      <c r="T53" s="1"/>
+      <c r="U53" s="1"/>
+      <c r="V53" s="1"/>
+      <c r="W53" s="1"/>
+      <c r="X53" s="1"/>
+      <c r="Y53" s="1"/>
+      <c r="Z53" s="1"/>
+      <c r="AA53" s="1"/>
+      <c r="AB53" s="1"/>
+      <c r="AC53" s="1"/>
+      <c r="AD53" s="1"/>
+      <c r="AE53" s="1"/>
+      <c r="AF53" s="1"/>
+      <c r="AG53" s="1"/>
+      <c r="AH53" s="1"/>
+      <c r="AI53" s="1"/>
     </row>
     <row r="54" ht="12.75" customHeight="1">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
-      <c r="C54" s="7"/>
-      <c r="D54" s="7"/>
-      <c r="E54" s="7"/>
-      <c r="F54" s="7"/>
-      <c r="G54" s="7"/>
-      <c r="H54" s="7"/>
-      <c r="I54" s="7"/>
-      <c r="J54" s="7"/>
-      <c r="K54" s="7"/>
-      <c r="L54" s="7"/>
-      <c r="M54" s="7"/>
-      <c r="N54" s="7"/>
-      <c r="O54" s="7"/>
-      <c r="P54" s="7"/>
-      <c r="Q54" s="7"/>
-      <c r="R54" s="7"/>
-      <c r="S54" s="7"/>
-      <c r="T54" s="7"/>
-      <c r="U54" s="7"/>
-      <c r="V54" s="7"/>
-      <c r="W54" s="7"/>
-      <c r="X54" s="7"/>
-      <c r="Y54" s="7"/>
-      <c r="Z54" s="7"/>
-      <c r="AA54" s="7"/>
-      <c r="AB54" s="7"/>
-      <c r="AC54" s="7"/>
-      <c r="AD54" s="7"/>
-      <c r="AE54" s="7"/>
-      <c r="AF54" s="7"/>
-      <c r="AG54" s="7"/>
-      <c r="AH54" s="7"/>
-      <c r="AI54" s="7"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
+      <c r="L54" s="1"/>
+      <c r="M54" s="1"/>
+      <c r="N54" s="1"/>
+      <c r="O54" s="1"/>
+      <c r="P54" s="1"/>
+      <c r="Q54" s="1"/>
+      <c r="R54" s="1"/>
+      <c r="S54" s="1"/>
+      <c r="T54" s="1"/>
+      <c r="U54" s="1"/>
+      <c r="V54" s="1"/>
+      <c r="W54" s="1"/>
+      <c r="X54" s="1"/>
+      <c r="Y54" s="1"/>
+      <c r="Z54" s="1"/>
+      <c r="AA54" s="1"/>
+      <c r="AB54" s="1"/>
+      <c r="AC54" s="1"/>
+      <c r="AD54" s="1"/>
+      <c r="AE54" s="1"/>
+      <c r="AF54" s="1"/>
+      <c r="AG54" s="1"/>
+      <c r="AH54" s="1"/>
+      <c r="AI54" s="1"/>
     </row>
     <row r="55" ht="12.75" customHeight="1">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
-      <c r="C55" s="7"/>
-      <c r="D55" s="7"/>
-      <c r="E55" s="7"/>
-      <c r="F55" s="7"/>
-      <c r="G55" s="7"/>
-      <c r="H55" s="7"/>
-      <c r="I55" s="7"/>
-      <c r="J55" s="7"/>
-      <c r="K55" s="7"/>
-      <c r="L55" s="7"/>
-      <c r="M55" s="7"/>
-      <c r="N55" s="7"/>
-      <c r="O55" s="7"/>
-      <c r="P55" s="7"/>
-      <c r="Q55" s="7"/>
-      <c r="R55" s="7"/>
-      <c r="S55" s="7"/>
-      <c r="T55" s="7"/>
-      <c r="U55" s="7"/>
-      <c r="V55" s="7"/>
-      <c r="W55" s="7"/>
-      <c r="X55" s="7"/>
-      <c r="Y55" s="7"/>
-      <c r="Z55" s="7"/>
-      <c r="AA55" s="7"/>
-      <c r="AB55" s="7"/>
-      <c r="AC55" s="7"/>
-      <c r="AD55" s="7"/>
-      <c r="AE55" s="7"/>
-      <c r="AF55" s="7"/>
-      <c r="AG55" s="7"/>
-      <c r="AH55" s="7"/>
-      <c r="AI55" s="7"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+      <c r="K55" s="1"/>
+      <c r="L55" s="1"/>
+      <c r="M55" s="1"/>
+      <c r="N55" s="1"/>
+      <c r="O55" s="1"/>
+      <c r="P55" s="1"/>
+      <c r="Q55" s="1"/>
+      <c r="R55" s="1"/>
+      <c r="S55" s="1"/>
+      <c r="T55" s="1"/>
+      <c r="U55" s="1"/>
+      <c r="V55" s="1"/>
+      <c r="W55" s="1"/>
+      <c r="X55" s="1"/>
+      <c r="Y55" s="1"/>
+      <c r="Z55" s="1"/>
+      <c r="AA55" s="1"/>
+      <c r="AB55" s="1"/>
+      <c r="AC55" s="1"/>
+      <c r="AD55" s="1"/>
+      <c r="AE55" s="1"/>
+      <c r="AF55" s="1"/>
+      <c r="AG55" s="1"/>
+      <c r="AH55" s="1"/>
+      <c r="AI55" s="1"/>
     </row>
     <row r="56" ht="12.75" customHeight="1">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
-      <c r="C56" s="7"/>
-      <c r="D56" s="7"/>
-      <c r="E56" s="7"/>
-      <c r="F56" s="7"/>
-      <c r="G56" s="7"/>
-      <c r="H56" s="7"/>
-      <c r="I56" s="7"/>
-      <c r="J56" s="7"/>
-      <c r="K56" s="7"/>
-      <c r="L56" s="7"/>
-      <c r="M56" s="7"/>
-      <c r="N56" s="7"/>
-      <c r="O56" s="7"/>
-      <c r="P56" s="7"/>
-      <c r="Q56" s="7"/>
-      <c r="R56" s="7"/>
-      <c r="S56" s="7"/>
-      <c r="T56" s="7"/>
-      <c r="U56" s="7"/>
-      <c r="V56" s="7"/>
-      <c r="W56" s="7"/>
-      <c r="X56" s="7"/>
-      <c r="Y56" s="7"/>
-      <c r="Z56" s="7"/>
-      <c r="AA56" s="7"/>
-      <c r="AB56" s="7"/>
-      <c r="AC56" s="7"/>
-      <c r="AD56" s="7"/>
-      <c r="AE56" s="7"/>
-      <c r="AF56" s="7"/>
-      <c r="AG56" s="7"/>
-      <c r="AH56" s="7"/>
-      <c r="AI56" s="7"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+      <c r="K56" s="1"/>
+      <c r="L56" s="1"/>
+      <c r="M56" s="1"/>
+      <c r="N56" s="1"/>
+      <c r="O56" s="1"/>
+      <c r="P56" s="1"/>
+      <c r="Q56" s="1"/>
+      <c r="R56" s="1"/>
+      <c r="S56" s="1"/>
+      <c r="T56" s="1"/>
+      <c r="U56" s="1"/>
+      <c r="V56" s="1"/>
+      <c r="W56" s="1"/>
+      <c r="X56" s="1"/>
+      <c r="Y56" s="1"/>
+      <c r="Z56" s="1"/>
+      <c r="AA56" s="1"/>
+      <c r="AB56" s="1"/>
+      <c r="AC56" s="1"/>
+      <c r="AD56" s="1"/>
+      <c r="AE56" s="1"/>
+      <c r="AF56" s="1"/>
+      <c r="AG56" s="1"/>
+      <c r="AH56" s="1"/>
+      <c r="AI56" s="1"/>
     </row>
     <row r="57" ht="12.75" customHeight="1">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
-      <c r="C57" s="7"/>
-      <c r="D57" s="7"/>
-      <c r="E57" s="7"/>
-      <c r="F57" s="7"/>
-      <c r="G57" s="7"/>
-      <c r="H57" s="7"/>
-      <c r="I57" s="7"/>
-      <c r="J57" s="7"/>
-      <c r="K57" s="7"/>
-      <c r="L57" s="7"/>
-      <c r="M57" s="7"/>
-      <c r="N57" s="7"/>
-      <c r="O57" s="7"/>
-      <c r="P57" s="7"/>
-      <c r="Q57" s="7"/>
-      <c r="R57" s="7"/>
-      <c r="S57" s="7"/>
-      <c r="T57" s="7"/>
-      <c r="U57" s="7"/>
-      <c r="V57" s="7"/>
-      <c r="W57" s="7"/>
-      <c r="X57" s="7"/>
-      <c r="Y57" s="7"/>
-      <c r="Z57" s="7"/>
-      <c r="AA57" s="7"/>
-      <c r="AB57" s="7"/>
-      <c r="AC57" s="7"/>
-      <c r="AD57" s="7"/>
-      <c r="AE57" s="7"/>
-      <c r="AF57" s="7"/>
-      <c r="AG57" s="7"/>
-      <c r="AH57" s="7"/>
-      <c r="AI57" s="7"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+      <c r="K57" s="1"/>
+      <c r="L57" s="1"/>
+      <c r="M57" s="1"/>
+      <c r="N57" s="1"/>
+      <c r="O57" s="1"/>
+      <c r="P57" s="1"/>
+      <c r="Q57" s="1"/>
+      <c r="R57" s="1"/>
+      <c r="S57" s="1"/>
+      <c r="T57" s="1"/>
+      <c r="U57" s="1"/>
+      <c r="V57" s="1"/>
+      <c r="W57" s="1"/>
+      <c r="X57" s="1"/>
+      <c r="Y57" s="1"/>
+      <c r="Z57" s="1"/>
+      <c r="AA57" s="1"/>
+      <c r="AB57" s="1"/>
+      <c r="AC57" s="1"/>
+      <c r="AD57" s="1"/>
+      <c r="AE57" s="1"/>
+      <c r="AF57" s="1"/>
+      <c r="AG57" s="1"/>
+      <c r="AH57" s="1"/>
+      <c r="AI57" s="1"/>
     </row>
     <row r="58" ht="12.75" customHeight="1">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
-      <c r="C58" s="7"/>
-      <c r="D58" s="7"/>
-      <c r="E58" s="7"/>
-      <c r="F58" s="7"/>
-      <c r="G58" s="7"/>
-      <c r="H58" s="7"/>
-      <c r="I58" s="7"/>
-      <c r="J58" s="7"/>
-      <c r="K58" s="7"/>
-      <c r="L58" s="7"/>
-      <c r="M58" s="7"/>
-      <c r="N58" s="7"/>
-      <c r="O58" s="7"/>
-      <c r="P58" s="7"/>
-      <c r="Q58" s="7"/>
-      <c r="R58" s="7"/>
-      <c r="S58" s="7"/>
-      <c r="T58" s="7"/>
-      <c r="U58" s="7"/>
-      <c r="V58" s="7"/>
-      <c r="W58" s="7"/>
-      <c r="X58" s="7"/>
-      <c r="Y58" s="7"/>
-      <c r="Z58" s="7"/>
-      <c r="AA58" s="7"/>
-      <c r="AB58" s="7"/>
-      <c r="AC58" s="7"/>
-      <c r="AD58" s="7"/>
-      <c r="AE58" s="7"/>
-      <c r="AF58" s="7"/>
-      <c r="AG58" s="7"/>
-      <c r="AH58" s="7"/>
-      <c r="AI58" s="7"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1"/>
+      <c r="L58" s="1"/>
+      <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
+      <c r="O58" s="1"/>
+      <c r="P58" s="1"/>
+      <c r="Q58" s="1"/>
+      <c r="R58" s="1"/>
+      <c r="S58" s="1"/>
+      <c r="T58" s="1"/>
+      <c r="U58" s="1"/>
+      <c r="V58" s="1"/>
+      <c r="W58" s="1"/>
+      <c r="X58" s="1"/>
+      <c r="Y58" s="1"/>
+      <c r="Z58" s="1"/>
+      <c r="AA58" s="1"/>
+      <c r="AB58" s="1"/>
+      <c r="AC58" s="1"/>
+      <c r="AD58" s="1"/>
+      <c r="AE58" s="1"/>
+      <c r="AF58" s="1"/>
+      <c r="AG58" s="1"/>
+      <c r="AH58" s="1"/>
+      <c r="AI58" s="1"/>
     </row>
     <row r="59" ht="12.75" customHeight="1">
       <c r="A59" s="1"/>
@@ -37345,235 +37135,13 @@
       <c r="AH983" s="1"/>
       <c r="AI983" s="1"/>
     </row>
-    <row r="984" ht="12.75" customHeight="1">
-      <c r="A984" s="1"/>
-      <c r="B984" s="1"/>
-      <c r="C984" s="1"/>
-      <c r="D984" s="1"/>
-      <c r="E984" s="1"/>
-      <c r="F984" s="1"/>
-      <c r="G984" s="1"/>
-      <c r="H984" s="1"/>
-      <c r="I984" s="1"/>
-      <c r="J984" s="1"/>
-      <c r="K984" s="1"/>
-      <c r="L984" s="1"/>
-      <c r="M984" s="1"/>
-      <c r="N984" s="1"/>
-      <c r="O984" s="1"/>
-      <c r="P984" s="1"/>
-      <c r="Q984" s="1"/>
-      <c r="R984" s="1"/>
-      <c r="S984" s="1"/>
-      <c r="T984" s="1"/>
-      <c r="U984" s="1"/>
-      <c r="V984" s="1"/>
-      <c r="W984" s="1"/>
-      <c r="X984" s="1"/>
-      <c r="Y984" s="1"/>
-      <c r="Z984" s="1"/>
-      <c r="AA984" s="1"/>
-      <c r="AB984" s="1"/>
-      <c r="AC984" s="1"/>
-      <c r="AD984" s="1"/>
-      <c r="AE984" s="1"/>
-      <c r="AF984" s="1"/>
-      <c r="AG984" s="1"/>
-      <c r="AH984" s="1"/>
-      <c r="AI984" s="1"/>
-    </row>
-    <row r="985" ht="12.75" customHeight="1">
-      <c r="A985" s="1"/>
-      <c r="B985" s="1"/>
-      <c r="C985" s="1"/>
-      <c r="D985" s="1"/>
-      <c r="E985" s="1"/>
-      <c r="F985" s="1"/>
-      <c r="G985" s="1"/>
-      <c r="H985" s="1"/>
-      <c r="I985" s="1"/>
-      <c r="J985" s="1"/>
-      <c r="K985" s="1"/>
-      <c r="L985" s="1"/>
-      <c r="M985" s="1"/>
-      <c r="N985" s="1"/>
-      <c r="O985" s="1"/>
-      <c r="P985" s="1"/>
-      <c r="Q985" s="1"/>
-      <c r="R985" s="1"/>
-      <c r="S985" s="1"/>
-      <c r="T985" s="1"/>
-      <c r="U985" s="1"/>
-      <c r="V985" s="1"/>
-      <c r="W985" s="1"/>
-      <c r="X985" s="1"/>
-      <c r="Y985" s="1"/>
-      <c r="Z985" s="1"/>
-      <c r="AA985" s="1"/>
-      <c r="AB985" s="1"/>
-      <c r="AC985" s="1"/>
-      <c r="AD985" s="1"/>
-      <c r="AE985" s="1"/>
-      <c r="AF985" s="1"/>
-      <c r="AG985" s="1"/>
-      <c r="AH985" s="1"/>
-      <c r="AI985" s="1"/>
-    </row>
-    <row r="986" ht="12.75" customHeight="1">
-      <c r="A986" s="1"/>
-      <c r="B986" s="1"/>
-      <c r="C986" s="1"/>
-      <c r="D986" s="1"/>
-      <c r="E986" s="1"/>
-      <c r="F986" s="1"/>
-      <c r="G986" s="1"/>
-      <c r="H986" s="1"/>
-      <c r="I986" s="1"/>
-      <c r="J986" s="1"/>
-      <c r="K986" s="1"/>
-      <c r="L986" s="1"/>
-      <c r="M986" s="1"/>
-      <c r="N986" s="1"/>
-      <c r="O986" s="1"/>
-      <c r="P986" s="1"/>
-      <c r="Q986" s="1"/>
-      <c r="R986" s="1"/>
-      <c r="S986" s="1"/>
-      <c r="T986" s="1"/>
-      <c r="U986" s="1"/>
-      <c r="V986" s="1"/>
-      <c r="W986" s="1"/>
-      <c r="X986" s="1"/>
-      <c r="Y986" s="1"/>
-      <c r="Z986" s="1"/>
-      <c r="AA986" s="1"/>
-      <c r="AB986" s="1"/>
-      <c r="AC986" s="1"/>
-      <c r="AD986" s="1"/>
-      <c r="AE986" s="1"/>
-      <c r="AF986" s="1"/>
-      <c r="AG986" s="1"/>
-      <c r="AH986" s="1"/>
-      <c r="AI986" s="1"/>
-    </row>
-    <row r="987" ht="12.75" customHeight="1">
-      <c r="A987" s="1"/>
-      <c r="B987" s="1"/>
-      <c r="C987" s="1"/>
-      <c r="D987" s="1"/>
-      <c r="E987" s="1"/>
-      <c r="F987" s="1"/>
-      <c r="G987" s="1"/>
-      <c r="H987" s="1"/>
-      <c r="I987" s="1"/>
-      <c r="J987" s="1"/>
-      <c r="K987" s="1"/>
-      <c r="L987" s="1"/>
-      <c r="M987" s="1"/>
-      <c r="N987" s="1"/>
-      <c r="O987" s="1"/>
-      <c r="P987" s="1"/>
-      <c r="Q987" s="1"/>
-      <c r="R987" s="1"/>
-      <c r="S987" s="1"/>
-      <c r="T987" s="1"/>
-      <c r="U987" s="1"/>
-      <c r="V987" s="1"/>
-      <c r="W987" s="1"/>
-      <c r="X987" s="1"/>
-      <c r="Y987" s="1"/>
-      <c r="Z987" s="1"/>
-      <c r="AA987" s="1"/>
-      <c r="AB987" s="1"/>
-      <c r="AC987" s="1"/>
-      <c r="AD987" s="1"/>
-      <c r="AE987" s="1"/>
-      <c r="AF987" s="1"/>
-      <c r="AG987" s="1"/>
-      <c r="AH987" s="1"/>
-      <c r="AI987" s="1"/>
-    </row>
-    <row r="988" ht="12.75" customHeight="1">
-      <c r="A988" s="1"/>
-      <c r="B988" s="1"/>
-      <c r="C988" s="1"/>
-      <c r="D988" s="1"/>
-      <c r="E988" s="1"/>
-      <c r="F988" s="1"/>
-      <c r="G988" s="1"/>
-      <c r="H988" s="1"/>
-      <c r="I988" s="1"/>
-      <c r="J988" s="1"/>
-      <c r="K988" s="1"/>
-      <c r="L988" s="1"/>
-      <c r="M988" s="1"/>
-      <c r="N988" s="1"/>
-      <c r="O988" s="1"/>
-      <c r="P988" s="1"/>
-      <c r="Q988" s="1"/>
-      <c r="R988" s="1"/>
-      <c r="S988" s="1"/>
-      <c r="T988" s="1"/>
-      <c r="U988" s="1"/>
-      <c r="V988" s="1"/>
-      <c r="W988" s="1"/>
-      <c r="X988" s="1"/>
-      <c r="Y988" s="1"/>
-      <c r="Z988" s="1"/>
-      <c r="AA988" s="1"/>
-      <c r="AB988" s="1"/>
-      <c r="AC988" s="1"/>
-      <c r="AD988" s="1"/>
-      <c r="AE988" s="1"/>
-      <c r="AF988" s="1"/>
-      <c r="AG988" s="1"/>
-      <c r="AH988" s="1"/>
-      <c r="AI988" s="1"/>
-    </row>
-    <row r="989" ht="12.75" customHeight="1">
-      <c r="A989" s="1"/>
-      <c r="B989" s="1"/>
-      <c r="C989" s="1"/>
-      <c r="D989" s="1"/>
-      <c r="E989" s="1"/>
-      <c r="F989" s="1"/>
-      <c r="G989" s="1"/>
-      <c r="H989" s="1"/>
-      <c r="I989" s="1"/>
-      <c r="J989" s="1"/>
-      <c r="K989" s="1"/>
-      <c r="L989" s="1"/>
-      <c r="M989" s="1"/>
-      <c r="N989" s="1"/>
-      <c r="O989" s="1"/>
-      <c r="P989" s="1"/>
-      <c r="Q989" s="1"/>
-      <c r="R989" s="1"/>
-      <c r="S989" s="1"/>
-      <c r="T989" s="1"/>
-      <c r="U989" s="1"/>
-      <c r="V989" s="1"/>
-      <c r="W989" s="1"/>
-      <c r="X989" s="1"/>
-      <c r="Y989" s="1"/>
-      <c r="Z989" s="1"/>
-      <c r="AA989" s="1"/>
-      <c r="AB989" s="1"/>
-      <c r="AC989" s="1"/>
-      <c r="AD989" s="1"/>
-      <c r="AE989" s="1"/>
-      <c r="AF989" s="1"/>
-      <c r="AG989" s="1"/>
-      <c r="AH989" s="1"/>
-      <c r="AI989" s="1"/>
-    </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="L3:L20">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="L3:L14">
       <formula1>Status</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="O5:O20">
-      <formula1>$A$14:$A$20</formula1>
+    <dataValidation type="list" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="O5:O14">
+      <formula1>$A$14</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions/>

</xml_diff>